<commit_message>
mario lau new data
</commit_message>
<xml_diff>
--- a/T_data数据汇总.xlsx
+++ b/T_data数据汇总.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelly Jinzhe Liu\Desktop\Big-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggary\Desktop\新增資料夾\Big-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7677E62E-D9A4-46C2-963D-AB9B1BF9CDB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D059FDF1-E42E-4E55-854B-69932FB65DAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -90,7 +90,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -114,7 +114,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -143,7 +143,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -159,13 +159,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -198,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -221,11 +221,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,9 +256,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -265,7 +277,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -302,7 +314,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-HK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -755,7 +767,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1550926719"/>
@@ -814,7 +826,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1550925471"/>
@@ -856,7 +868,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-HK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -893,7 +905,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-HK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1764,18 +1776,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1804,7 +1816,7 @@
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +1893,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:26">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1958,7 +1970,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:26">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1966,76 +1978,77 @@
         <v>77.5</v>
       </c>
       <c r="C4" s="5">
-        <v>75.8</v>
+        <v>69.3</v>
       </c>
       <c r="D4" s="5">
-        <v>72.400000000000006</v>
+        <v>60.1</v>
       </c>
       <c r="E4" s="5">
+        <v>51.4</v>
+      </c>
+      <c r="F4" s="5">
+        <v>52.9</v>
+      </c>
+      <c r="G4" s="5">
+        <v>55.1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>56.8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>58.7</v>
+      </c>
+      <c r="J4" s="5">
+        <v>62.5</v>
+      </c>
+      <c r="K4" s="5">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="L4" s="5">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="M4" s="5">
+        <v>66.7</v>
+      </c>
+      <c r="N4" s="5">
+        <v>67.5</v>
+      </c>
+      <c r="O4" s="5">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="P4" s="5">
+        <v>67.3</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="R4" s="5">
+        <v>67.7</v>
+      </c>
+      <c r="S4" s="5">
+        <v>69.2</v>
+      </c>
+      <c r="T4" s="5">
         <v>71.099999999999994</v>
       </c>
-      <c r="F4" s="5">
-        <v>70.3</v>
-      </c>
-      <c r="G4" s="5">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="H4" s="5">
-        <v>67.400000000000006</v>
-      </c>
-      <c r="I4" s="5">
-        <v>67.3</v>
-      </c>
-      <c r="J4" s="5">
-        <v>67.2</v>
-      </c>
-      <c r="K4" s="5">
-        <v>67</v>
-      </c>
-      <c r="L4" s="5">
-        <v>66.900000000000006</v>
-      </c>
-      <c r="M4" s="5">
-        <v>66.8</v>
-      </c>
-      <c r="N4" s="5">
-        <v>66.400000000000006</v>
-      </c>
-      <c r="O4" s="5">
-        <v>66.38</v>
-      </c>
-      <c r="P4" s="5">
-        <v>66.349999999999994</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>66.3</v>
-      </c>
-      <c r="R4" s="5">
-        <v>66.260000000000005</v>
-      </c>
-      <c r="S4" s="5">
-        <v>66.150000000000006</v>
-      </c>
-      <c r="T4" s="5">
-        <v>66.099999999999994</v>
-      </c>
       <c r="U4" s="5">
-        <v>66.03</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="V4" s="5">
-        <v>65.900000000000006</v>
+        <v>72.3</v>
       </c>
       <c r="W4" s="5">
-        <v>65.599999999999994</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="X4" s="5">
-        <v>65.3</v>
+        <v>73.5</v>
       </c>
       <c r="Y4" s="5">
-        <v>65.099999999999994</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="Z4" s="9"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:26">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2112,7 +2125,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:26">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -2189,7 +2202,7 @@
         <v>10902</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:26">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2266,10 +2279,10 @@
         <v>82958</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:26">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:26">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2296,7 +2309,7 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:26">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2323,19 +2336,19 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:26">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:26">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:26">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:26">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:26">
       <c r="A15" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mario matplot graph basic version
</commit_message>
<xml_diff>
--- a/T_data数据汇总.xlsx
+++ b/T_data数据汇总.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelly Jinzhe Liu\Desktop\Big-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggary\Desktop\新增資料夾\Big-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7C6D6E-C4F3-4F06-8A19-EFF00E3CE4E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011344B8-393F-46E5-8D25-4EDF6D80B075}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4770" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -90,7 +90,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -114,7 +114,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -143,7 +143,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -159,13 +159,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -259,7 +259,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -277,7 +277,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -330,13 +330,13 @@
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2000000000000002</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0999999999999996</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.2000000000000002</c:v>
@@ -345,7 +345,7 @@
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0999999999999996</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.2</c:v>
@@ -375,19 +375,19 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1999999999999993</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8.1</c:v>
@@ -411,13 +411,13 @@
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2000000000000002</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0999999999999996</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.2000000000000002</c:v>
@@ -426,7 +426,7 @@
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0999999999999996</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.2</c:v>
@@ -456,19 +456,19 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1999999999999993</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8.1</c:v>
@@ -525,13 +525,13 @@
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2000000000000002</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0999999999999996</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.2000000000000002</c:v>
@@ -540,7 +540,7 @@
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0999999999999996</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.2</c:v>
@@ -570,19 +570,19 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1999999999999993</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8.1</c:v>
@@ -720,13 +720,13 @@
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2000000000000002</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0999999999999996</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.2000000000000002</c:v>
@@ -735,7 +735,7 @@
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0999999999999996</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.2</c:v>
@@ -765,19 +765,19 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1999999999999993</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8.1</c:v>
@@ -929,7 +929,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="404428127"/>
@@ -988,7 +988,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="404427711"/>
@@ -1036,7 +1036,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-HK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1050,7 +1050,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1087,7 +1087,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-HK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1143,13 +1143,13 @@
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2000000000000002</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0999999999999996</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.2000000000000002</c:v>
@@ -1158,7 +1158,7 @@
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0999999999999996</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.2</c:v>
@@ -1188,19 +1188,19 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1999999999999993</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8.1</c:v>
@@ -1355,7 +1355,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="405152703"/>
@@ -1414,7 +1414,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="405153119"/>
@@ -1462,7 +1462,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-HK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1476,7 +1476,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1513,7 +1513,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-HK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1559,13 +1559,13 @@
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2000000000000002</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0999999999999996</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.2000000000000002</c:v>
@@ -1574,7 +1574,7 @@
                   <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0999999999999996</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.2</c:v>
@@ -1604,19 +1604,19 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1999999999999993</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8.1</c:v>
@@ -1771,7 +1771,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="464956239"/>
@@ -1830,7 +1830,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-HK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="464951247"/>
@@ -1878,7 +1878,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-HK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3935,11 +3935,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45.42578125" customWidth="1"/>
   </cols>
@@ -3981,13 +3981,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="4">
-        <v>1.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="D2" s="4">
         <v>1.3</v>
       </c>
       <c r="E2" s="4">
-        <v>2.0999999999999996</v>
+        <v>2.1</v>
       </c>
       <c r="F2" s="4">
         <v>2.2000000000000002</v>
@@ -3996,7 +3996,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H2" s="4">
-        <v>3.0999999999999996</v>
+        <v>3.1</v>
       </c>
       <c r="I2" s="4">
         <v>3.2</v>
@@ -4026,19 +4026,19 @@
         <v>6.1</v>
       </c>
       <c r="R2" s="4">
-        <v>6.1999999999999993</v>
+        <v>6.2</v>
       </c>
       <c r="S2" s="4">
-        <v>6.3000000000000007</v>
+        <v>6.3</v>
       </c>
       <c r="T2" s="4">
         <v>7.1</v>
       </c>
       <c r="U2" s="4">
-        <v>7.1999999999999993</v>
+        <v>7.2</v>
       </c>
       <c r="V2" s="4">
-        <v>7.3000000000000007</v>
+        <v>7.3</v>
       </c>
       <c r="W2" s="4">
         <v>8.1</v>

</xml_diff>